<commit_message>
fixed 2c cluster index problem and tested data
</commit_message>
<xml_diff>
--- a/Data/real_data.xlsx
+++ b/Data/real_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/304b24243408c27c/Desktop/projects/Salesforce/SalesForceProject/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{95D339D6-2EDE-114E-BBDB-B55B126DB7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9A11663-5552-4D62-A5AF-6269DD4229C7}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{95D339D6-2EDE-114E-BBDB-B55B126DB7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C498B939-B527-49F6-8553-95DE3FE61DFC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9AC16B38-AC6A-BB4A-A160-B32F658F594D}"/>
   </bookViews>
@@ -9409,7 +9409,7 @@
   <dimension ref="A1:F1501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>